<commit_message>
Versión del planteo entregada
</commit_message>
<xml_diff>
--- a/Planteo y simulación manual.xlsx
+++ b/Planteo y simulación manual.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\TP4-Simulacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\GitHub\TP4-Simulacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0E5900-24B1-49C8-BFC5-1C25C4978F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECC49A7-4963-4E55-B775-9234F5C22B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{12BCEDD2-8242-4AFC-A31D-5713CDD2C3D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{12BCEDD2-8242-4AFC-A31D-5713CDD2C3D8}"/>
   </bookViews>
   <sheets>
-    <sheet name="TP4" sheetId="1" r:id="rId1"/>
+    <sheet name="TP4" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="INFO A PRESENTAR" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -900,7 +900,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="157">
   <si>
     <t>Fin ControlComida i</t>
   </si>
@@ -1131,12 +1131,6 @@
   </si>
   <si>
     <t>Tiempo en conseguir entrada</t>
-  </si>
-  <si>
-    <t>Promedio de metros necesarios para aparcamiento</t>
-  </si>
-  <si>
-    <t>Unidad</t>
   </si>
   <si>
     <t>Tiempo de entrada despues de estacionar</t>
@@ -1189,27 +1183,9 @@
     </r>
   </si>
   <si>
-    <t>Contando la suma de los metros de cada auto dividido la cantidad total de autos.</t>
-  </si>
-  <si>
-    <t>Minutos</t>
-  </si>
-  <si>
     <t>VECTOR ESTADO</t>
   </si>
   <si>
-    <t>PromedioMetros</t>
-  </si>
-  <si>
-    <t>TiempoEntrada</t>
-  </si>
-  <si>
-    <t>TiempoEntradaDespEstacionar</t>
-  </si>
-  <si>
-    <t>Sumatoria de (Cantidad de personas en cola por el tiempo en que hay esa cantidad de personas en cola), dividido el reloj de la simulación</t>
-  </si>
-  <si>
     <t>Exponencial negativa</t>
   </si>
   <si>
@@ -1225,60 +1201,15 @@
     <t>Constante</t>
   </si>
   <si>
-    <t>CantidadPromedioGenteEnCola</t>
-  </si>
-  <si>
     <t>COMO LO CALCULA?</t>
   </si>
   <si>
-    <t>PORQUE LO CALCULA</t>
-  </si>
-  <si>
-    <t>En cada experimento de la simulación</t>
-  </si>
-  <si>
     <t>DÓNDE LO CALCULA ?</t>
   </si>
   <si>
-    <t xml:space="preserve">Porque necesitamos buscar el dato de cuantas personas en promedio hay en cola, por lo tanto se toma este acumulador para poder calcularlo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se suma uno una vez que haya sucedido el evento de la llegada cliente </t>
-  </si>
-  <si>
-    <t>AcumuladorColaEntrada</t>
-  </si>
-  <si>
-    <t>Cantidad promedio de gente en ColaEntrada</t>
-  </si>
-  <si>
-    <t>AcumuladorTiempo</t>
-  </si>
-  <si>
-    <t>Se suma el tiempo anterior de espera en cola al tiempo actual de espera en cola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porque necesitamos buscar el dato de cuanto tiempo hubo una cierta cantidad de personas en cola, por lo tanto se toma este acumulador para poder calcularlo </t>
-  </si>
-  <si>
-    <t>AcumuladorTiempo A CHEQUEAAAAAR</t>
-  </si>
-  <si>
     <t>ACUMULADORES Y CONTADORES</t>
   </si>
   <si>
-    <t>ContadorAutos</t>
-  </si>
-  <si>
-    <t>Por cada auto que llega se suma 1 al contador</t>
-  </si>
-  <si>
-    <t>Porque necesitamos buscar el promedio de metros necesarios para aparcamiento y para ello necesitamos la cantidad total de datos.</t>
-  </si>
-  <si>
-    <t>A CHEQUEAAR</t>
-  </si>
-  <si>
     <t>HoraFinCajaPark</t>
   </si>
   <si>
@@ -1324,9 +1255,6 @@
     <t>Servidor       ControlComida (i)</t>
   </si>
   <si>
-    <t>Servidor        ContorlComidaMayores(i)</t>
-  </si>
-  <si>
     <t>(i)</t>
   </si>
   <si>
@@ -1348,7 +1276,145 @@
     <t>Hora Cola entrada</t>
   </si>
   <si>
-    <t>Sumamos 5 minutos + [(RND de cola entrada*60) (minutos en cola entrada)* Cantidad de personas en colaEntrada]</t>
+    <t>300 + Tiempo promedio en colaEntrada + 92</t>
+  </si>
+  <si>
+    <t>Tiempo promedio en colaEntrada*</t>
+  </si>
+  <si>
+    <t>* Métrica auxiliar</t>
+  </si>
+  <si>
+    <t>(Sumatoria de tiempos en colaEntrada / Tiempo total de la simulación) * 4,16</t>
+  </si>
+  <si>
+    <t>4,16: Cantidad promedio de personas por grupo</t>
+  </si>
+  <si>
+    <t>Unidades</t>
+  </si>
+  <si>
+    <t>Tiempo en conseguir entrada + Tiempo promedio en colaComida + 5</t>
+  </si>
+  <si>
+    <t>5: Tiempo promedio de atención en ControlComida</t>
+  </si>
+  <si>
+    <t>300: 5 minutos, 92: Tiempo promedio de atención en CajaEntrada</t>
+  </si>
+  <si>
+    <t>Tiempo promedio en colaComida*</t>
+  </si>
+  <si>
+    <t>Cantidad promedio de autos en colaPark*</t>
+  </si>
+  <si>
+    <t>Cantidad promedio de autos en colaPark * 4. ALTERNATIVA: Cantidad máxima de autos en la colaPark * 4</t>
+  </si>
+  <si>
+    <t>(Sumatoria de tiempos en colaParking / Tiempo total de la simulación)</t>
+  </si>
+  <si>
+    <t>Metros promedio necesarios para aparcamiento</t>
+  </si>
+  <si>
+    <t>POR QUÉ LO CALCULA?</t>
+  </si>
+  <si>
+    <t>SumatoriaTiemposColaParking</t>
+  </si>
+  <si>
+    <t>CantidadMaximaAutosEnColaParking</t>
+  </si>
+  <si>
+    <t>SumatoriaTiemposColaEntrada</t>
+  </si>
+  <si>
+    <t>ContadorGruposQuePasaronPorCajaEntrada</t>
+  </si>
+  <si>
+    <t>Sumatoria de tiempos en colaEntrada / Cantidad de grupos que pasaron por las CajaEntrada</t>
+  </si>
+  <si>
+    <t>SumatoriaTiemposColaComida</t>
+  </si>
+  <si>
+    <t>ContadorGruposQuePasaronPorControlComida</t>
+  </si>
+  <si>
+    <t>Sumatoria de tiempos en colaComida / Cantidad de grupos que pasaron por los ControlComida</t>
+  </si>
+  <si>
+    <t>Se calcula con la función MAX(), tomando como parámetros la cantidad máxima anterior, y la cantidad de autos en colaParking actual. Devuelve el mayor valor entre estos dos parámetros.</t>
+  </si>
+  <si>
+    <t>En cada evento de la simulación</t>
+  </si>
+  <si>
+    <t>Se requiere para la solución alternativa de la estadística: Metros promedio necesarios para aparcamiento.</t>
+  </si>
+  <si>
+    <t>i = 1, 2,.., 20</t>
+  </si>
+  <si>
+    <t>Servidor        ControlComidaMayores</t>
+  </si>
+  <si>
+    <t>Se calcula sumando todos los tiempos de colaParking de los autos en el momento actual, más la suma anterior.</t>
+  </si>
+  <si>
+    <t>Se requiere para la estadística: Cantidad promedio de autos en colaPark.</t>
+  </si>
+  <si>
+    <t>Se calcula sumando todos los tiempos de colaEntrada de los grupos en el momento actual, más la suma anterior.</t>
+  </si>
+  <si>
+    <t>Se calcula sumando 1 por cada grupo que ejecuta el evento FinCajaEntrada.</t>
+  </si>
+  <si>
+    <t>Se requiere para la estadística: Tiempo promedio en colaEntrada.</t>
+  </si>
+  <si>
+    <t>Se calcula sumando todos los tiempos de colaComida de las personas en el momento actual, más la suma anterior.</t>
+  </si>
+  <si>
+    <t>Se requiere para la estadística: Tiempo promedio en colaComida.</t>
+  </si>
+  <si>
+    <t>Se requiere para la estadística: Tiempo promedio en colaEntrada y Cantidad promedio de gente en colaEntrada.</t>
+  </si>
+  <si>
+    <t>Cantidad promedio de gente en colaEntrada</t>
+  </si>
+  <si>
+    <t>Se calcula sumando 1 por cada persona que ejecuta el evento FinControlComida.</t>
+  </si>
+  <si>
+    <t>CantidadMaxima AutosEnColaParking</t>
+  </si>
+  <si>
+    <t>SumatoriaTiempos ColaParking</t>
+  </si>
+  <si>
+    <t>SumatoriaTiempos ColaEntrada</t>
+  </si>
+  <si>
+    <t>ContadorGruposQue PasaronPorCajaEntrada</t>
+  </si>
+  <si>
+    <t>SumatoriaTiempos ColaComida</t>
+  </si>
+  <si>
+    <t>ContadorGruposQue PasaronPorControlComida</t>
+  </si>
+  <si>
+    <t>Llegada</t>
+  </si>
+  <si>
+    <t>Estadísticas</t>
+  </si>
+  <si>
+    <t>Objetos temporales</t>
   </si>
 </sst>
 </file>
@@ -1416,7 +1482,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1480,12 +1546,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1624,7 +1684,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1709,64 +1769,97 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1774,9 +1867,6 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1786,57 +1876,49 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2162,76 +2244,76 @@
   <dimension ref="A1:BF51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17" customWidth="1"/>
-    <col min="25" max="25" width="14.1796875" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
       <c r="F1" s="31"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
       <c r="O1" s="22"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49"/>
-      <c r="AA1" s="49"/>
-      <c r="AB1" s="49"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="52"/>
-      <c r="AV1" s="52"/>
-      <c r="AW1" s="52"/>
-      <c r="AX1" s="52"/>
-      <c r="AY1" s="52"/>
-      <c r="AZ1" s="52"/>
-      <c r="BA1" s="52"/>
-      <c r="BB1" s="52"/>
-      <c r="BC1" s="52"/>
-      <c r="BD1" s="52"/>
-      <c r="BE1" s="52"/>
-      <c r="BF1" s="52"/>
-    </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.35">
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="45"/>
+      <c r="AF1" s="45"/>
+      <c r="AG1" s="45"/>
+      <c r="AH1" s="45"/>
+      <c r="AI1" s="45"/>
+      <c r="AJ1" s="45"/>
+      <c r="AK1" s="45"/>
+      <c r="AL1" s="45"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="38"/>
+      <c r="AR1" s="38"/>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38"/>
+      <c r="AU1" s="39"/>
+      <c r="AV1" s="39"/>
+      <c r="AW1" s="39"/>
+      <c r="AX1" s="39"/>
+      <c r="AY1" s="39"/>
+      <c r="AZ1" s="39"/>
+      <c r="BA1" s="39"/>
+      <c r="BB1" s="39"/>
+      <c r="BC1" s="39"/>
+      <c r="BD1" s="39"/>
+      <c r="BE1" s="39"/>
+      <c r="BF1" s="39"/>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B2" s="34" t="s">
         <v>36</v>
       </c>
@@ -2265,62 +2347,62 @@
       <c r="Z2" s="23"/>
       <c r="AA2" s="23"/>
       <c r="AB2" s="23"/>
-      <c r="AC2" s="45">
+      <c r="AC2" s="46">
         <v>1</v>
       </c>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="45">
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="46">
         <v>2</v>
       </c>
-      <c r="AF2" s="46"/>
-      <c r="AG2" s="45">
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="46">
         <v>3</v>
       </c>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="45">
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="46">
         <v>4</v>
       </c>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="45">
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="46">
         <v>5</v>
       </c>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="43">
+      <c r="AL2" s="45"/>
+      <c r="AM2" s="41">
         <v>1</v>
       </c>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="43">
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="41">
         <v>2</v>
       </c>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="43">
+      <c r="AP2" s="38"/>
+      <c r="AQ2" s="41">
         <v>3</v>
       </c>
-      <c r="AR2" s="44"/>
-      <c r="AS2" s="43">
+      <c r="AR2" s="38"/>
+      <c r="AS2" s="41">
         <v>4</v>
       </c>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="56">
+      <c r="AT2" s="38"/>
+      <c r="AU2" s="40">
         <v>1</v>
       </c>
-      <c r="AV2" s="52"/>
-      <c r="AW2" s="52"/>
-      <c r="AX2" s="52"/>
-      <c r="AY2" s="56">
+      <c r="AV2" s="39"/>
+      <c r="AW2" s="39"/>
+      <c r="AX2" s="39"/>
+      <c r="AY2" s="40">
         <v>2</v>
       </c>
-      <c r="AZ2" s="52"/>
-      <c r="BA2" s="52"/>
-      <c r="BB2" s="52"/>
-      <c r="BC2" s="56">
+      <c r="AZ2" s="39"/>
+      <c r="BA2" s="39"/>
+      <c r="BB2" s="39"/>
+      <c r="BC2" s="40">
         <v>3</v>
       </c>
-      <c r="BD2" s="52"/>
-      <c r="BE2" s="52"/>
-      <c r="BF2" s="52"/>
-    </row>
-    <row r="3" spans="1:58" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BD2" s="39"/>
+      <c r="BE2" s="39"/>
+      <c r="BF2" s="39"/>
+    </row>
+    <row r="3" spans="1:58" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>35</v>
       </c>
@@ -2450,7 +2532,7 @@
       <c r="BE3" s="9"/>
       <c r="BF3" s="9"/>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2460,7 +2542,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2471,7 +2553,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2482,7 +2564,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -2494,7 +2576,7 @@
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2514,7 +2596,7 @@
       <c r="AB8" s="4"/>
       <c r="AP8" s="4"/>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2530,7 +2612,7 @@
       <c r="AB9" s="4"/>
       <c r="AC9" s="4"/>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2543,7 +2625,7 @@
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
@@ -2553,7 +2635,7 @@
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
@@ -2566,7 +2648,7 @@
       <c r="AK12" s="4"/>
       <c r="AL12" s="4"/>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -2579,7 +2661,7 @@
       <c r="AK13" s="4"/>
       <c r="AL13" s="4"/>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="5"/>
@@ -2591,7 +2673,7 @@
       <c r="AK14" s="4"/>
       <c r="AL14" s="4"/>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -2602,7 +2684,7 @@
       <c r="AB15" s="4"/>
       <c r="AL15" s="4"/>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -2614,7 +2696,7 @@
       <c r="AP16" s="4"/>
       <c r="BB16" s="4"/>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="F17" s="5"/>
       <c r="I17" s="4"/>
@@ -2624,43 +2706,43 @@
       <c r="AK17" s="4"/>
       <c r="AL17" s="4"/>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="I18" s="4"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="21" spans="1:38" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:38" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="R21" s="47" t="s">
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42"/>
+      <c r="R21" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
-      <c r="U21" s="47"/>
-      <c r="V21" s="47"/>
+      <c r="S21" s="42"/>
+      <c r="T21" s="42"/>
+      <c r="U21" s="42"/>
+      <c r="V21" s="42"/>
       <c r="X21" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:38" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0.67</v>
       </c>
@@ -2684,15 +2766,15 @@
       <c r="T22" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="U22" s="42" t="s">
+      <c r="U22" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="V22" s="42"/>
+      <c r="V22" s="52"/>
       <c r="Y22" s="35" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.23</v>
       </c>
@@ -2741,7 +2823,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.89</v>
       </c>
@@ -2768,7 +2850,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.45</v>
       </c>
@@ -2791,7 +2873,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.02</v>
       </c>
@@ -2802,7 +2884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.76</v>
       </c>
@@ -2810,135 +2892,135 @@
       <c r="R27" s="2"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.54</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.11</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.87</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.32</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.61</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.08</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.93</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.39</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.78</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.48</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.06</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.83</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.27</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.94</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.51</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.18</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.63</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.35</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.81</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.42</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.97</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0.69</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AM1:AT1"/>
-    <mergeCell ref="AU1:BF1"/>
-    <mergeCell ref="BC2:BF2"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AU2:AX2"/>
-    <mergeCell ref="AY2:BB2"/>
-    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
     <mergeCell ref="C21:P21"/>
     <mergeCell ref="R21:V21"/>
     <mergeCell ref="V1:W1"/>
@@ -2951,13 +3033,13 @@
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AM1:AT1"/>
+    <mergeCell ref="AU1:BF1"/>
+    <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AU2:AX2"/>
+    <mergeCell ref="AY2:BB2"/>
+    <mergeCell ref="AQ2:AR2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -2967,69 +3049,68 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6241246C-E157-40C2-A22D-12210E17A066}">
-  <dimension ref="A1:AK44"/>
+  <dimension ref="A1:AJ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI47" sqref="AI47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.26953125" customWidth="1"/>
-    <col min="2" max="2" width="41.7265625" customWidth="1"/>
-    <col min="3" max="3" width="121.81640625" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" customWidth="1"/>
-    <col min="22" max="22" width="14.1796875" customWidth="1"/>
-    <col min="23" max="23" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+    <col min="3" max="3" width="121.85546875" customWidth="1"/>
+    <col min="4" max="4" width="47.5703125" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" customWidth="1"/>
+    <col min="23" max="23" width="19.42578125" customWidth="1"/>
     <col min="24" max="24" width="19" customWidth="1"/>
-    <col min="25" max="25" width="23.453125" customWidth="1"/>
-    <col min="26" max="26" width="14.26953125" customWidth="1"/>
-    <col min="27" max="27" width="14.453125" customWidth="1"/>
-    <col min="28" max="28" width="29.54296875" customWidth="1"/>
-    <col min="29" max="29" width="21.81640625" customWidth="1"/>
+    <col min="25" max="25" width="23.42578125" customWidth="1"/>
+    <col min="26" max="26" width="26.28515625" customWidth="1"/>
+    <col min="27" max="27" width="22.85546875" customWidth="1"/>
+    <col min="28" max="28" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="E1" s="49" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="E1" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="s">
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="E2" s="67" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="E2" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="65"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>44</v>
       </c>
@@ -3039,14 +3120,14 @@
       <c r="C6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="67" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D6" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -3056,12 +3137,12 @@
       <c r="C7" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3071,12 +3152,12 @@
       <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3086,12 +3167,12 @@
       <c r="C9" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -3101,12 +3182,12 @@
       <c r="C10" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3116,12 +3197,12 @@
       <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3131,12 +3212,12 @@
       <c r="C12" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3146,12 +3227,12 @@
       <c r="C13" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -3162,7 +3243,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>54</v>
       </c>
@@ -3173,51 +3254,52 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17">
+        <v>84</v>
+      </c>
+      <c r="C17" s="34">
         <v>0.66659999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="D18" s="87"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>61</v>
       </c>
@@ -3228,7 +3310,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -3239,7 +3321,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -3250,7 +3332,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -3261,7 +3343,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -3272,7 +3354,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>67</v>
       </c>
@@ -3282,399 +3364,551 @@
       <c r="C28" s="23" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="B29" t="s">
         <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>76</v>
       </c>
-      <c r="B30" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="37" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="D38" s="73" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="73" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" s="73" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" s="73" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="73" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A44" s="37"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="74"/>
+    </row>
+    <row r="45" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="L46" s="57"/>
+      <c r="M46" s="57"/>
+      <c r="N46" s="57"/>
+      <c r="O46" s="57"/>
+      <c r="P46" s="57"/>
+      <c r="Q46" s="57"/>
+      <c r="R46" s="57"/>
+      <c r="S46" s="57"/>
+      <c r="T46" s="57"/>
+      <c r="U46" s="57"/>
+      <c r="V46" s="57"/>
+      <c r="W46" s="57"/>
+      <c r="X46" s="57"/>
+      <c r="Y46" s="57"/>
+      <c r="Z46" s="57"/>
+      <c r="AA46" s="57"/>
+      <c r="AB46" s="57"/>
+      <c r="AC46" s="57"/>
+      <c r="AD46" s="57"/>
+      <c r="AE46" s="57"/>
+      <c r="AF46" s="57"/>
+      <c r="AG46" s="57"/>
+      <c r="AH46" s="57"/>
+      <c r="AI46" s="57"/>
+      <c r="AJ46" s="58"/>
+    </row>
+    <row r="47" spans="1:36" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="75"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="81" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="81"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="G47" s="82"/>
+      <c r="H47" s="82"/>
+      <c r="I47" s="83" t="s">
+        <v>58</v>
+      </c>
+      <c r="J47" s="83"/>
+      <c r="K47" s="83"/>
+      <c r="L47" s="84" t="s">
+        <v>59</v>
+      </c>
+      <c r="M47" s="84"/>
+      <c r="N47" s="84"/>
+      <c r="O47" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="P47" s="76"/>
+      <c r="Q47" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="R47" s="77"/>
+      <c r="S47" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="T47" s="78"/>
+      <c r="U47" s="79"/>
+      <c r="V47" s="79"/>
+      <c r="W47" s="85" t="s">
+        <v>155</v>
+      </c>
+      <c r="X47" s="85"/>
+      <c r="Y47" s="85"/>
+      <c r="Z47" s="85"/>
+      <c r="AA47" s="85"/>
+      <c r="AB47" s="85"/>
+      <c r="AC47" s="86" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD47" s="86"/>
+      <c r="AE47" s="86"/>
+      <c r="AF47" s="86"/>
+      <c r="AG47" s="86"/>
+      <c r="AH47" s="86"/>
+      <c r="AI47" s="86"/>
+      <c r="AJ47" s="86"/>
+    </row>
+    <row r="48" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="E48" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="F48" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="G48" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="H48" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="I48" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="J48" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="K48" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="L48" s="69" t="s">
+        <v>93</v>
+      </c>
+      <c r="M48" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="N48" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="O48" s="70" t="s">
+        <v>100</v>
+      </c>
+      <c r="P48" s="70"/>
+      <c r="Q48" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A34" s="23" t="s">
+      <c r="R48" s="71"/>
+      <c r="S48" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="T48" s="72"/>
+      <c r="U48" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="V48" s="63"/>
+      <c r="W48" s="80" t="s">
+        <v>148</v>
+      </c>
+      <c r="X48" s="80" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y48" s="80" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z48" s="80" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA48" s="80" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB48" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC48" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD48" s="64"/>
+      <c r="AE48" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:37" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="D35" s="37" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:37" ht="116" x14ac:dyDescent="0.35">
-      <c r="A36" s="39" t="s">
+      <c r="AF48" s="64"/>
+      <c r="AG48" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="AH48" s="45"/>
+      <c r="AI48" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="AJ48" s="45"/>
+    </row>
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A49" s="60"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="68"/>
+      <c r="J49" s="68"/>
+      <c r="K49" s="68"/>
+      <c r="L49" s="69"/>
+      <c r="M49" s="69"/>
+      <c r="N49" s="69"/>
+      <c r="O49" s="70"/>
+      <c r="P49" s="70"/>
+      <c r="Q49" s="71"/>
+      <c r="R49" s="71"/>
+      <c r="S49" s="72"/>
+      <c r="T49" s="72"/>
+      <c r="U49" s="63"/>
+      <c r="V49" s="63"/>
+      <c r="W49" s="80"/>
+      <c r="X49" s="80"/>
+      <c r="Y49" s="80"/>
+      <c r="Z49" s="80"/>
+      <c r="AA49" s="80"/>
+      <c r="AB49" s="80"/>
+      <c r="AC49" s="65" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" s="41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:37" ht="87" x14ac:dyDescent="0.35">
-      <c r="A37" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="B37" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="D37" s="36" t="s">
+      <c r="AD49" s="66"/>
+      <c r="AE49" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF49" s="45"/>
+      <c r="AG49" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH49" s="45"/>
+      <c r="AI49" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="AJ49" s="45"/>
+    </row>
+    <row r="50" spans="1:36" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="60"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="67"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="68"/>
+      <c r="J50" s="68"/>
+      <c r="K50" s="68"/>
+      <c r="L50" s="69"/>
+      <c r="M50" s="69"/>
+      <c r="N50" s="69"/>
+      <c r="O50" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="P50" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q50" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="R50" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="S50" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="T50" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="U50" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="V50" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="W50" s="80"/>
+      <c r="X50" s="80"/>
+      <c r="Y50" s="80"/>
+      <c r="Z50" s="80"/>
+      <c r="AA50" s="80"/>
+      <c r="AB50" s="80"/>
+      <c r="AC50" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD50" s="13"/>
+      <c r="AE50" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF50" s="13" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="41" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="77" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="78"/>
-      <c r="C41" s="78"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
-      <c r="H41" s="78"/>
-      <c r="I41" s="78"/>
-      <c r="J41" s="78"/>
-      <c r="K41" s="78"/>
-      <c r="L41" s="78"/>
-      <c r="M41" s="78"/>
-      <c r="N41" s="78"/>
-      <c r="O41" s="78"/>
-      <c r="P41" s="78"/>
-      <c r="Q41" s="78"/>
-      <c r="R41" s="78"/>
-      <c r="S41" s="78"/>
-      <c r="T41" s="78"/>
-      <c r="U41" s="78"/>
-      <c r="V41" s="78"/>
-      <c r="W41" s="78"/>
-      <c r="X41" s="78"/>
-      <c r="Y41" s="78"/>
-      <c r="Z41" s="78"/>
-      <c r="AA41" s="78"/>
-      <c r="AB41" s="78"/>
-      <c r="AC41" s="78"/>
-      <c r="AD41" s="78"/>
-      <c r="AE41" s="78"/>
-      <c r="AF41" s="78"/>
-      <c r="AG41" s="78"/>
-      <c r="AH41" s="78"/>
-      <c r="AI41" s="78"/>
-      <c r="AJ41" s="78"/>
-      <c r="AK41" s="79"/>
-    </row>
-    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="73" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="75" t="s">
-        <v>132</v>
-      </c>
-      <c r="C42" s="66" t="s">
-        <v>120</v>
-      </c>
-      <c r="D42" s="66" t="s">
-        <v>121</v>
-      </c>
-      <c r="E42" s="66" t="s">
-        <v>122</v>
-      </c>
-      <c r="F42" s="57" t="s">
-        <v>111</v>
-      </c>
-      <c r="G42" s="57" t="s">
-        <v>112</v>
-      </c>
-      <c r="H42" s="57" t="s">
-        <v>113</v>
-      </c>
-      <c r="I42" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="J42" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="K42" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="L42" s="59" t="s">
-        <v>116</v>
-      </c>
-      <c r="M42" s="59" t="s">
-        <v>117</v>
-      </c>
-      <c r="N42" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="O42" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="P42" s="60"/>
-      <c r="Q42" s="61" t="s">
-        <v>124</v>
-      </c>
-      <c r="R42" s="61"/>
-      <c r="S42" s="62" t="s">
-        <v>125</v>
-      </c>
-      <c r="T42" s="62"/>
-      <c r="U42" s="63" t="s">
-        <v>126</v>
-      </c>
-      <c r="V42" s="63"/>
-      <c r="W42" s="64" t="s">
-        <v>107</v>
-      </c>
-      <c r="X42" s="64" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y42" s="64" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z42" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA42" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB42" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC42" s="69" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD42" s="70" t="s">
-        <v>131</v>
-      </c>
-      <c r="AE42" s="70"/>
-      <c r="AF42" s="70" t="s">
-        <v>130</v>
-      </c>
-      <c r="AG42" s="70"/>
-      <c r="AH42" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="AI42" s="46"/>
-      <c r="AJ42" s="46" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK42" s="46"/>
-    </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A43" s="74"/>
-      <c r="B43" s="76"/>
-      <c r="C43" s="66"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="66"/>
-      <c r="F43" s="57"/>
-      <c r="G43" s="57"/>
-      <c r="H43" s="57"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="58"/>
-      <c r="L43" s="59"/>
-      <c r="M43" s="59"/>
-      <c r="N43" s="59"/>
-      <c r="O43" s="60"/>
-      <c r="P43" s="60"/>
-      <c r="Q43" s="61"/>
-      <c r="R43" s="61"/>
-      <c r="S43" s="62"/>
-      <c r="T43" s="62"/>
-      <c r="U43" s="63"/>
-      <c r="V43" s="63"/>
-      <c r="W43" s="64"/>
-      <c r="X43" s="64"/>
-      <c r="Y43" s="64"/>
-      <c r="Z43" s="68"/>
-      <c r="AA43" s="68"/>
-      <c r="AB43" s="69"/>
-      <c r="AC43" s="69"/>
-      <c r="AD43" s="71" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE43" s="72"/>
-      <c r="AF43" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG43" s="46"/>
-      <c r="AH43" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="AI43" s="46"/>
-      <c r="AJ43" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK43" s="46"/>
-    </row>
-    <row r="44" spans="1:37" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="74"/>
-      <c r="B44" s="76"/>
-      <c r="C44" s="66"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
-      <c r="K44" s="58"/>
-      <c r="L44" s="59"/>
-      <c r="M44" s="59"/>
-      <c r="N44" s="59"/>
-      <c r="O44" s="19" t="s">
+      <c r="AG50" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="P44" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q44" s="18" t="s">
+      <c r="AH50" s="13"/>
+      <c r="AI50" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="R44" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="S44" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="T44" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="U44" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="V44" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="W44" s="64"/>
-      <c r="X44" s="64"/>
-      <c r="Y44" s="64"/>
-      <c r="Z44" s="68"/>
-      <c r="AA44" s="68"/>
-      <c r="AB44" s="69"/>
-      <c r="AC44" s="69"/>
-      <c r="AD44" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE44" s="13"/>
-      <c r="AF44" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="AG44" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="AH44" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI44" s="13"/>
-      <c r="AJ44" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="AK44" s="13"/>
+      <c r="AJ50" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="48">
+    <mergeCell ref="W47:AB47"/>
+    <mergeCell ref="AC47:AJ47"/>
+    <mergeCell ref="U47:V47"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="Q48:R49"/>
+    <mergeCell ref="S48:T49"/>
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="S47:T47"/>
+    <mergeCell ref="K48:K50"/>
+    <mergeCell ref="L48:L50"/>
+    <mergeCell ref="M48:M50"/>
+    <mergeCell ref="N48:N50"/>
+    <mergeCell ref="O48:P49"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="G48:G50"/>
+    <mergeCell ref="H48:H50"/>
+    <mergeCell ref="I48:I50"/>
+    <mergeCell ref="J48:J50"/>
+    <mergeCell ref="AG48:AH48"/>
+    <mergeCell ref="AI48:AJ48"/>
+    <mergeCell ref="AC49:AD49"/>
+    <mergeCell ref="AE49:AF49"/>
+    <mergeCell ref="AG49:AH49"/>
+    <mergeCell ref="AI49:AJ49"/>
+    <mergeCell ref="AA48:AA50"/>
+    <mergeCell ref="AB48:AB50"/>
+    <mergeCell ref="AC48:AD48"/>
+    <mergeCell ref="AE48:AF48"/>
     <mergeCell ref="A2:C4"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="E48:E50"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E2:G4"/>
     <mergeCell ref="D6:G13"/>
-    <mergeCell ref="A41:AK41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="U42:V43"/>
-    <mergeCell ref="W42:W44"/>
-    <mergeCell ref="X42:X44"/>
-    <mergeCell ref="Y42:Y44"/>
-    <mergeCell ref="Z42:Z44"/>
-    <mergeCell ref="AA42:AA44"/>
-    <mergeCell ref="AB42:AB44"/>
-    <mergeCell ref="AC42:AC44"/>
-    <mergeCell ref="AD42:AE42"/>
-    <mergeCell ref="AF42:AG42"/>
-    <mergeCell ref="AH42:AI42"/>
-    <mergeCell ref="AJ42:AK42"/>
-    <mergeCell ref="AD43:AE43"/>
-    <mergeCell ref="AF43:AG43"/>
-    <mergeCell ref="AH43:AI43"/>
-    <mergeCell ref="AJ43:AK43"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="I42:I44"/>
-    <mergeCell ref="J42:J44"/>
-    <mergeCell ref="K42:K44"/>
-    <mergeCell ref="L42:L44"/>
-    <mergeCell ref="M42:M44"/>
-    <mergeCell ref="N42:N44"/>
-    <mergeCell ref="O42:P43"/>
-    <mergeCell ref="Q42:R43"/>
-    <mergeCell ref="S42:T43"/>
+    <mergeCell ref="A46:AJ46"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="U48:V49"/>
+    <mergeCell ref="W48:W50"/>
+    <mergeCell ref="X48:X50"/>
+    <mergeCell ref="Y48:Y50"/>
+    <mergeCell ref="Z48:Z50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Creación del proyecto + pseudo
</commit_message>
<xml_diff>
--- a/Planteo y simulación manual.xlsx
+++ b/Planteo y simulación manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\GitHub\TP4-Simulacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolás\Documents\GitHub\TP4-Simulacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECC49A7-4963-4E55-B775-9234F5C22B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CA9843-AB04-43F0-B709-5CADE3230B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{12BCEDD2-8242-4AFC-A31D-5713CDD2C3D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{12BCEDD2-8242-4AFC-A31D-5713CDD2C3D8}"/>
   </bookViews>
   <sheets>
     <sheet name="TP4" sheetId="1" state="hidden" r:id="rId1"/>
@@ -900,7 +900,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="154">
   <si>
     <t>Fin ControlComida i</t>
   </si>
@@ -1309,9 +1309,6 @@
     <t>Cantidad promedio de autos en colaPark*</t>
   </si>
   <si>
-    <t>Cantidad promedio de autos en colaPark * 4. ALTERNATIVA: Cantidad máxima de autos en la colaPark * 4</t>
-  </si>
-  <si>
     <t>(Sumatoria de tiempos en colaParking / Tiempo total de la simulación)</t>
   </si>
   <si>
@@ -1324,9 +1321,6 @@
     <t>SumatoriaTiemposColaParking</t>
   </si>
   <si>
-    <t>CantidadMaximaAutosEnColaParking</t>
-  </si>
-  <si>
     <t>SumatoriaTiemposColaEntrada</t>
   </si>
   <si>
@@ -1339,21 +1333,12 @@
     <t>SumatoriaTiemposColaComida</t>
   </si>
   <si>
-    <t>ContadorGruposQuePasaronPorControlComida</t>
-  </si>
-  <si>
     <t>Sumatoria de tiempos en colaComida / Cantidad de grupos que pasaron por los ControlComida</t>
   </si>
   <si>
-    <t>Se calcula con la función MAX(), tomando como parámetros la cantidad máxima anterior, y la cantidad de autos en colaParking actual. Devuelve el mayor valor entre estos dos parámetros.</t>
-  </si>
-  <si>
     <t>En cada evento de la simulación</t>
   </si>
   <si>
-    <t>Se requiere para la solución alternativa de la estadística: Metros promedio necesarios para aparcamiento.</t>
-  </si>
-  <si>
     <t>i = 1, 2,.., 20</t>
   </si>
   <si>
@@ -1415,6 +1400,12 @@
   </si>
   <si>
     <t>Objetos temporales</t>
+  </si>
+  <si>
+    <t>ContadorPersonasQuePasaronPorControlComida</t>
+  </si>
+  <si>
+    <t>Cantidad promedio de autos en colaPark * 4.</t>
   </si>
 </sst>
 </file>
@@ -1684,7 +1675,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1771,50 +1762,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1849,76 +1909,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2256,32 +2246,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="31"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
       <c r="O1" s="22"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
       <c r="AC1" s="45"/>
       <c r="AD1" s="45"/>
       <c r="AE1" s="45"/>
@@ -2292,26 +2282,26 @@
       <c r="AJ1" s="45"/>
       <c r="AK1" s="45"/>
       <c r="AL1" s="45"/>
-      <c r="AM1" s="38"/>
-      <c r="AN1" s="38"/>
-      <c r="AO1" s="38"/>
-      <c r="AP1" s="38"/>
-      <c r="AQ1" s="38"/>
-      <c r="AR1" s="38"/>
-      <c r="AS1" s="38"/>
-      <c r="AT1" s="38"/>
-      <c r="AU1" s="39"/>
-      <c r="AV1" s="39"/>
-      <c r="AW1" s="39"/>
-      <c r="AX1" s="39"/>
-      <c r="AY1" s="39"/>
-      <c r="AZ1" s="39"/>
-      <c r="BA1" s="39"/>
-      <c r="BB1" s="39"/>
-      <c r="BC1" s="39"/>
-      <c r="BD1" s="39"/>
-      <c r="BE1" s="39"/>
-      <c r="BF1" s="39"/>
+      <c r="AM1" s="43"/>
+      <c r="AN1" s="43"/>
+      <c r="AO1" s="43"/>
+      <c r="AP1" s="43"/>
+      <c r="AQ1" s="43"/>
+      <c r="AR1" s="43"/>
+      <c r="AS1" s="43"/>
+      <c r="AT1" s="43"/>
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="51"/>
+      <c r="AW1" s="51"/>
+      <c r="AX1" s="51"/>
+      <c r="AY1" s="51"/>
+      <c r="AZ1" s="51"/>
+      <c r="BA1" s="51"/>
+      <c r="BB1" s="51"/>
+      <c r="BC1" s="51"/>
+      <c r="BD1" s="51"/>
+      <c r="BE1" s="51"/>
+      <c r="BF1" s="51"/>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B2" s="34" t="s">
@@ -2347,60 +2337,60 @@
       <c r="Z2" s="23"/>
       <c r="AA2" s="23"/>
       <c r="AB2" s="23"/>
-      <c r="AC2" s="46">
+      <c r="AC2" s="44">
         <v>1</v>
       </c>
       <c r="AD2" s="45"/>
-      <c r="AE2" s="46">
+      <c r="AE2" s="44">
         <v>2</v>
       </c>
       <c r="AF2" s="45"/>
-      <c r="AG2" s="46">
+      <c r="AG2" s="44">
         <v>3</v>
       </c>
       <c r="AH2" s="45"/>
-      <c r="AI2" s="46">
+      <c r="AI2" s="44">
         <v>4</v>
       </c>
       <c r="AJ2" s="45"/>
-      <c r="AK2" s="46">
+      <c r="AK2" s="44">
         <v>5</v>
       </c>
       <c r="AL2" s="45"/>
-      <c r="AM2" s="41">
+      <c r="AM2" s="42">
         <v>1</v>
       </c>
-      <c r="AN2" s="38"/>
-      <c r="AO2" s="41">
+      <c r="AN2" s="43"/>
+      <c r="AO2" s="42">
         <v>2</v>
       </c>
-      <c r="AP2" s="38"/>
-      <c r="AQ2" s="41">
+      <c r="AP2" s="43"/>
+      <c r="AQ2" s="42">
         <v>3</v>
       </c>
-      <c r="AR2" s="38"/>
-      <c r="AS2" s="41">
+      <c r="AR2" s="43"/>
+      <c r="AS2" s="42">
         <v>4</v>
       </c>
-      <c r="AT2" s="38"/>
-      <c r="AU2" s="40">
+      <c r="AT2" s="43"/>
+      <c r="AU2" s="55">
         <v>1</v>
       </c>
-      <c r="AV2" s="39"/>
-      <c r="AW2" s="39"/>
-      <c r="AX2" s="39"/>
-      <c r="AY2" s="40">
+      <c r="AV2" s="51"/>
+      <c r="AW2" s="51"/>
+      <c r="AX2" s="51"/>
+      <c r="AY2" s="55">
         <v>2</v>
       </c>
-      <c r="AZ2" s="39"/>
-      <c r="BA2" s="39"/>
-      <c r="BB2" s="39"/>
-      <c r="BC2" s="40">
+      <c r="AZ2" s="51"/>
+      <c r="BA2" s="51"/>
+      <c r="BB2" s="51"/>
+      <c r="BC2" s="55">
         <v>3</v>
       </c>
-      <c r="BD2" s="39"/>
-      <c r="BE2" s="39"/>
-      <c r="BF2" s="39"/>
+      <c r="BD2" s="51"/>
+      <c r="BE2" s="51"/>
+      <c r="BF2" s="51"/>
     </row>
     <row r="3" spans="1:58" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -2715,29 +2705,29 @@
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
-      <c r="R21" s="42" t="s">
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="R21" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="S21" s="42"/>
-      <c r="T21" s="42"/>
-      <c r="U21" s="42"/>
-      <c r="V21" s="42"/>
+      <c r="S21" s="46"/>
+      <c r="T21" s="46"/>
+      <c r="U21" s="46"/>
+      <c r="V21" s="46"/>
       <c r="X21" s="3" t="s">
         <v>20</v>
       </c>
@@ -2766,10 +2756,10 @@
       <c r="T22" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="U22" s="52" t="s">
+      <c r="U22" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="V22" s="52"/>
+      <c r="V22" s="41"/>
       <c r="Y22" s="35" t="s">
         <v>40</v>
       </c>
@@ -3014,13 +3004,13 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AM1:AT1"/>
+    <mergeCell ref="AU1:BF1"/>
+    <mergeCell ref="BC2:BF2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AU2:AX2"/>
+    <mergeCell ref="AY2:BB2"/>
+    <mergeCell ref="AQ2:AR2"/>
     <mergeCell ref="C21:P21"/>
     <mergeCell ref="R21:V21"/>
     <mergeCell ref="V1:W1"/>
@@ -3033,13 +3023,13 @@
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="AM1:AT1"/>
-    <mergeCell ref="AU1:BF1"/>
-    <mergeCell ref="BC2:BF2"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AU2:AX2"/>
-    <mergeCell ref="AY2:BB2"/>
-    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3049,10 +3039,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6241246C-E157-40C2-A22D-12210E17A066}">
-  <dimension ref="A1:AJ50"/>
+  <dimension ref="A1:AJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3071,44 +3061,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="E1" s="44" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="E1" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="E2" s="55" t="s">
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="E2" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
+      <c r="A3" s="76"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
+      <c r="A4" s="76"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
@@ -3120,12 +3110,12 @@
       <c r="C6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3137,10 +3127,10 @@
       <c r="C7" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -3152,10 +3142,10 @@
       <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -3167,10 +3157,10 @@
       <c r="C9" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3182,10 +3172,10 @@
       <c r="C10" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -3197,10 +3187,10 @@
       <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -3212,10 +3202,10 @@
       <c r="C12" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -3227,10 +3217,10 @@
       <c r="C13" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -3275,7 +3265,6 @@
       <c r="C18" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="87"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -3370,13 +3359,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
         <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3387,7 +3376,7 @@
         <v>115</v>
       </c>
       <c r="C30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3412,12 +3401,12 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B33" t="s">
         <v>115</v>
@@ -3451,7 +3440,7 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
@@ -3465,21 +3454,21 @@
         <v>86</v>
       </c>
       <c r="D37" s="23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="37" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="38" spans="1:36" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
-        <v>126</v>
       </c>
       <c r="B38" s="36" t="s">
         <v>133</v>
       </c>
       <c r="C38" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="D38" s="38" t="s">
         <v>134</v>
-      </c>
-      <c r="D38" s="73" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:36" ht="45" x14ac:dyDescent="0.25">
@@ -3487,428 +3476,414 @@
         <v>125</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="D39" s="73" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="40" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="D39" s="38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="D40" s="73" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="37" t="s">
         <v>128</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C41" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="D41" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D41" s="38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="36" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="42" spans="1:36" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
+      <c r="C42" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="B42" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="C42" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="D42" s="73" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:36" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="s">
+      <c r="D42" s="38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A43" s="37"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="39"/>
+    </row>
+    <row r="44" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="80"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="80"/>
+      <c r="F45" s="80"/>
+      <c r="G45" s="80"/>
+      <c r="H45" s="80"/>
+      <c r="I45" s="80"/>
+      <c r="J45" s="80"/>
+      <c r="K45" s="80"/>
+      <c r="L45" s="80"/>
+      <c r="M45" s="80"/>
+      <c r="N45" s="80"/>
+      <c r="O45" s="80"/>
+      <c r="P45" s="80"/>
+      <c r="Q45" s="80"/>
+      <c r="R45" s="80"/>
+      <c r="S45" s="80"/>
+      <c r="T45" s="80"/>
+      <c r="U45" s="80"/>
+      <c r="V45" s="80"/>
+      <c r="W45" s="80"/>
+      <c r="X45" s="80"/>
+      <c r="Y45" s="80"/>
+      <c r="Z45" s="80"/>
+      <c r="AA45" s="80"/>
+      <c r="AB45" s="80"/>
+      <c r="AC45" s="80"/>
+      <c r="AD45" s="80"/>
+      <c r="AE45" s="80"/>
+      <c r="AF45" s="80"/>
+      <c r="AG45" s="80"/>
+      <c r="AH45" s="80"/>
+      <c r="AI45" s="80"/>
+      <c r="AJ45" s="81"/>
+    </row>
+    <row r="46" spans="1:36" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="G46" s="60"/>
+      <c r="H46" s="60"/>
+      <c r="I46" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="J46" s="61"/>
+      <c r="K46" s="61"/>
+      <c r="L46" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="M46" s="62"/>
+      <c r="N46" s="62"/>
+      <c r="O46" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="B43" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="C43" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="73" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A44" s="37"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="74"/>
-    </row>
-    <row r="45" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="57"/>
-      <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="57"/>
-      <c r="M46" s="57"/>
-      <c r="N46" s="57"/>
-      <c r="O46" s="57"/>
-      <c r="P46" s="57"/>
-      <c r="Q46" s="57"/>
-      <c r="R46" s="57"/>
-      <c r="S46" s="57"/>
-      <c r="T46" s="57"/>
-      <c r="U46" s="57"/>
-      <c r="V46" s="57"/>
-      <c r="W46" s="57"/>
-      <c r="X46" s="57"/>
-      <c r="Y46" s="57"/>
-      <c r="Z46" s="57"/>
-      <c r="AA46" s="57"/>
-      <c r="AB46" s="57"/>
-      <c r="AC46" s="57"/>
+      <c r="P46" s="65"/>
+      <c r="Q46" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="R46" s="66"/>
+      <c r="S46" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="T46" s="67"/>
+      <c r="U46" s="58"/>
+      <c r="V46" s="58"/>
+      <c r="W46" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="X46" s="56"/>
+      <c r="Y46" s="56"/>
+      <c r="Z46" s="56"/>
+      <c r="AA46" s="56"/>
+      <c r="AB46" s="56"/>
+      <c r="AC46" s="57" t="s">
+        <v>151</v>
+      </c>
       <c r="AD46" s="57"/>
       <c r="AE46" s="57"/>
       <c r="AF46" s="57"/>
       <c r="AG46" s="57"/>
       <c r="AH46" s="57"/>
       <c r="AI46" s="57"/>
-      <c r="AJ46" s="58"/>
-    </row>
-    <row r="47" spans="1:36" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="75"/>
-      <c r="B47" s="75"/>
-      <c r="C47" s="81" t="s">
-        <v>154</v>
-      </c>
-      <c r="D47" s="81"/>
-      <c r="E47" s="81"/>
-      <c r="F47" s="82" t="s">
-        <v>57</v>
-      </c>
-      <c r="G47" s="82"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="83" t="s">
-        <v>58</v>
-      </c>
-      <c r="J47" s="83"/>
-      <c r="K47" s="83"/>
-      <c r="L47" s="84" t="s">
-        <v>59</v>
-      </c>
-      <c r="M47" s="84"/>
-      <c r="N47" s="84"/>
-      <c r="O47" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="P47" s="76"/>
-      <c r="Q47" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="R47" s="77"/>
-      <c r="S47" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="T47" s="78"/>
-      <c r="U47" s="79"/>
-      <c r="V47" s="79"/>
-      <c r="W47" s="85" t="s">
-        <v>155</v>
-      </c>
-      <c r="X47" s="85"/>
-      <c r="Y47" s="85"/>
-      <c r="Z47" s="85"/>
-      <c r="AA47" s="85"/>
-      <c r="AB47" s="85"/>
-      <c r="AC47" s="86" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD47" s="86"/>
-      <c r="AE47" s="86"/>
-      <c r="AF47" s="86"/>
-      <c r="AG47" s="86"/>
-      <c r="AH47" s="86"/>
-      <c r="AI47" s="86"/>
-      <c r="AJ47" s="86"/>
-    </row>
-    <row r="48" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="59" t="s">
+      <c r="AJ46" s="57"/>
+    </row>
+    <row r="47" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="B48" s="61" t="s">
+      <c r="B47" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="C48" s="54" t="s">
+      <c r="C47" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="D48" s="54" t="s">
+      <c r="D47" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="E48" s="54" t="s">
+      <c r="E47" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="F48" s="67" t="s">
+      <c r="F47" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="G48" s="67" t="s">
+      <c r="G47" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="H48" s="67" t="s">
+      <c r="H47" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="I48" s="68" t="s">
+      <c r="I47" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="J48" s="68" t="s">
+      <c r="J47" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="K48" s="68" t="s">
+      <c r="K47" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="L48" s="69" t="s">
+      <c r="L47" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="M48" s="69" t="s">
+      <c r="M47" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="N48" s="69" t="s">
+      <c r="N47" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="O48" s="70" t="s">
+      <c r="O47" s="70" t="s">
         <v>100</v>
       </c>
+      <c r="P47" s="70"/>
+      <c r="Q47" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="R47" s="63"/>
+      <c r="S47" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="T47" s="64"/>
+      <c r="U47" s="86" t="s">
+        <v>132</v>
+      </c>
+      <c r="V47" s="86"/>
+      <c r="W47" s="74" t="s">
+        <v>143</v>
+      </c>
+      <c r="X47" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y47" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z47" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA47" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB47" s="74" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC47" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD47" s="75"/>
+      <c r="AE47" s="75" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF47" s="75"/>
+      <c r="AG47" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH47" s="45"/>
+      <c r="AI47" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="AJ47" s="45"/>
+    </row>
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A48" s="83"/>
+      <c r="B48" s="85"/>
+      <c r="C48" s="77"/>
+      <c r="D48" s="77"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="71"/>
+      <c r="G48" s="71"/>
+      <c r="H48" s="71"/>
+      <c r="I48" s="68"/>
+      <c r="J48" s="68"/>
+      <c r="K48" s="68"/>
+      <c r="L48" s="69"/>
+      <c r="M48" s="69"/>
+      <c r="N48" s="69"/>
+      <c r="O48" s="70"/>
       <c r="P48" s="70"/>
-      <c r="Q48" s="71" t="s">
-        <v>101</v>
-      </c>
-      <c r="R48" s="71"/>
-      <c r="S48" s="72" t="s">
-        <v>102</v>
-      </c>
-      <c r="T48" s="72"/>
-      <c r="U48" s="63" t="s">
-        <v>137</v>
-      </c>
-      <c r="V48" s="63"/>
-      <c r="W48" s="80" t="s">
-        <v>148</v>
-      </c>
-      <c r="X48" s="80" t="s">
-        <v>149</v>
-      </c>
-      <c r="Y48" s="80" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z48" s="80" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA48" s="80" t="s">
-        <v>152</v>
-      </c>
-      <c r="AB48" s="80" t="s">
-        <v>153</v>
-      </c>
-      <c r="AC48" s="64" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD48" s="64"/>
-      <c r="AE48" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF48" s="64"/>
-      <c r="AG48" s="45" t="s">
-        <v>105</v>
+      <c r="Q48" s="63"/>
+      <c r="R48" s="63"/>
+      <c r="S48" s="64"/>
+      <c r="T48" s="64"/>
+      <c r="U48" s="86"/>
+      <c r="V48" s="86"/>
+      <c r="W48" s="74"/>
+      <c r="X48" s="74"/>
+      <c r="Y48" s="74"/>
+      <c r="Z48" s="74"/>
+      <c r="AA48" s="74"/>
+      <c r="AB48" s="74"/>
+      <c r="AC48" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD48" s="73"/>
+      <c r="AE48" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF48" s="45"/>
+      <c r="AG48" s="44" t="s">
+        <v>103</v>
       </c>
       <c r="AH48" s="45"/>
-      <c r="AI48" s="45" t="s">
-        <v>104</v>
+      <c r="AI48" s="44" t="s">
+        <v>103</v>
       </c>
       <c r="AJ48" s="45"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A49" s="60"/>
-      <c r="B49" s="62"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="54"/>
-      <c r="E49" s="54"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="67"/>
-      <c r="H49" s="67"/>
+    <row r="49" spans="1:36" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="83"/>
+      <c r="B49" s="85"/>
+      <c r="C49" s="77"/>
+      <c r="D49" s="77"/>
+      <c r="E49" s="77"/>
+      <c r="F49" s="71"/>
+      <c r="G49" s="71"/>
+      <c r="H49" s="71"/>
       <c r="I49" s="68"/>
       <c r="J49" s="68"/>
       <c r="K49" s="68"/>
       <c r="L49" s="69"/>
       <c r="M49" s="69"/>
       <c r="N49" s="69"/>
-      <c r="O49" s="70"/>
-      <c r="P49" s="70"/>
-      <c r="Q49" s="71"/>
-      <c r="R49" s="71"/>
-      <c r="S49" s="72"/>
-      <c r="T49" s="72"/>
-      <c r="U49" s="63"/>
-      <c r="V49" s="63"/>
-      <c r="W49" s="80"/>
-      <c r="X49" s="80"/>
-      <c r="Y49" s="80"/>
-      <c r="Z49" s="80"/>
-      <c r="AA49" s="80"/>
-      <c r="AB49" s="80"/>
-      <c r="AC49" s="65" t="s">
-        <v>103</v>
-      </c>
-      <c r="AD49" s="66"/>
-      <c r="AE49" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF49" s="45"/>
-      <c r="AG49" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="AH49" s="45"/>
-      <c r="AI49" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="AJ49" s="45"/>
-    </row>
-    <row r="50" spans="1:36" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="60"/>
-      <c r="B50" s="62"/>
-      <c r="C50" s="54"/>
-      <c r="D50" s="54"/>
-      <c r="E50" s="54"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="67"/>
-      <c r="H50" s="67"/>
-      <c r="I50" s="68"/>
-      <c r="J50" s="68"/>
-      <c r="K50" s="68"/>
-      <c r="L50" s="69"/>
-      <c r="M50" s="69"/>
-      <c r="N50" s="69"/>
-      <c r="O50" s="19" t="s">
+      <c r="O49" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="P50" s="19" t="s">
+      <c r="P49" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="Q50" s="18" t="s">
+      <c r="Q49" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="R50" s="18" t="s">
+      <c r="R49" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="S50" s="17" t="s">
+      <c r="S49" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="T50" s="17" t="s">
+      <c r="T49" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="U50" s="16" t="s">
+      <c r="U49" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="V50" s="16" t="s">
+      <c r="V49" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="W50" s="80"/>
-      <c r="X50" s="80"/>
-      <c r="Y50" s="80"/>
-      <c r="Z50" s="80"/>
-      <c r="AA50" s="80"/>
-      <c r="AB50" s="80"/>
-      <c r="AC50" s="14" t="s">
+      <c r="W49" s="74"/>
+      <c r="X49" s="74"/>
+      <c r="Y49" s="74"/>
+      <c r="Z49" s="74"/>
+      <c r="AA49" s="74"/>
+      <c r="AB49" s="74"/>
+      <c r="AC49" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AD50" s="13"/>
-      <c r="AE50" s="14" t="s">
+      <c r="AD49" s="13"/>
+      <c r="AE49" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AF50" s="13" t="s">
+      <c r="AF49" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="AG50" s="14" t="s">
+      <c r="AG49" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AH50" s="13"/>
-      <c r="AI50" s="14" t="s">
+      <c r="AH49" s="13"/>
+      <c r="AI49" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AJ50" s="13"/>
+      <c r="AJ49" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="W47:AB47"/>
-    <mergeCell ref="AC47:AJ47"/>
-    <mergeCell ref="U47:V47"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="L47:N47"/>
-    <mergeCell ref="Q48:R49"/>
-    <mergeCell ref="S48:T49"/>
-    <mergeCell ref="O47:P47"/>
-    <mergeCell ref="Q47:R47"/>
-    <mergeCell ref="S47:T47"/>
-    <mergeCell ref="K48:K50"/>
-    <mergeCell ref="L48:L50"/>
-    <mergeCell ref="M48:M50"/>
-    <mergeCell ref="N48:N50"/>
-    <mergeCell ref="O48:P49"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="G48:G50"/>
-    <mergeCell ref="H48:H50"/>
-    <mergeCell ref="I48:I50"/>
-    <mergeCell ref="J48:J50"/>
-    <mergeCell ref="AG48:AH48"/>
-    <mergeCell ref="AI48:AJ48"/>
-    <mergeCell ref="AC49:AD49"/>
-    <mergeCell ref="AE49:AF49"/>
-    <mergeCell ref="AG49:AH49"/>
-    <mergeCell ref="AI49:AJ49"/>
-    <mergeCell ref="AA48:AA50"/>
-    <mergeCell ref="AB48:AB50"/>
-    <mergeCell ref="AC48:AD48"/>
-    <mergeCell ref="AE48:AF48"/>
-    <mergeCell ref="A2:C4"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="E48:E50"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E2:G4"/>
     <mergeCell ref="D6:G13"/>
-    <mergeCell ref="A46:AJ46"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="U48:V49"/>
-    <mergeCell ref="W48:W50"/>
-    <mergeCell ref="X48:X50"/>
-    <mergeCell ref="Y48:Y50"/>
-    <mergeCell ref="Z48:Z50"/>
+    <mergeCell ref="A45:AJ45"/>
+    <mergeCell ref="AA47:AA49"/>
+    <mergeCell ref="AB47:AB49"/>
+    <mergeCell ref="AC47:AD47"/>
+    <mergeCell ref="AE47:AF47"/>
+    <mergeCell ref="A2:C4"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="U47:V48"/>
+    <mergeCell ref="W47:W49"/>
+    <mergeCell ref="X47:X49"/>
+    <mergeCell ref="Y47:Y49"/>
+    <mergeCell ref="Z47:Z49"/>
+    <mergeCell ref="AG47:AH47"/>
+    <mergeCell ref="AI47:AJ47"/>
+    <mergeCell ref="AC48:AD48"/>
+    <mergeCell ref="AE48:AF48"/>
+    <mergeCell ref="AG48:AH48"/>
+    <mergeCell ref="AI48:AJ48"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="I47:I49"/>
+    <mergeCell ref="J47:J49"/>
+    <mergeCell ref="K47:K49"/>
+    <mergeCell ref="L47:L49"/>
+    <mergeCell ref="M47:M49"/>
+    <mergeCell ref="N47:N49"/>
+    <mergeCell ref="O47:P48"/>
+    <mergeCell ref="Q47:R48"/>
+    <mergeCell ref="S47:T48"/>
+    <mergeCell ref="O46:P46"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="S46:T46"/>
+    <mergeCell ref="W46:AB46"/>
+    <mergeCell ref="AC46:AJ46"/>
+    <mergeCell ref="U46:V46"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="L46:N46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>